<commit_message>
actualización general del proyecto
</commit_message>
<xml_diff>
--- a/apoyo/Historias de Usuario.xlsx
+++ b/apoyo/Historias de Usuario.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joseorellanaaravena/Documents/Full Stack JavaScript/06. Proyecto/alma/apoyo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1160FB-1605-6346-8975-1D5C8CE4F480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D06729-6F5C-304C-82F7-904CAD952A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{75795DB6-672D-E14C-B603-AE79CCF2FD41}"/>
   </bookViews>
@@ -576,8 +576,8 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>